<commit_message>
Updates 12S reference database and phyloseq code
</commit_message>
<xml_diff>
--- a/WADE003-arcticpred-12SP1-taxa-output-130trunc5.xlsx
+++ b/WADE003-arcticpred-12SP1-taxa-output-130trunc5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AA6F2D-FC6C-469D-8192-2F2D9D34001C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1698,20 +1698,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2613,12 +2613,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>120</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>122</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>123</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>125</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>129</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>130</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>131</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>132</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>133</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>134</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>135</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>136</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>137</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>138</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>139</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>141</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>142</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>144</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>148</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>149</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>150</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>151</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>152</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>154</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>155</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>156</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>157</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>158</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>159</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>160</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>161</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>162</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>163</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>164</v>
       </c>
@@ -4035,12 +4035,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>166</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>167</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>168</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>169</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>170</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>171</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>172</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>173</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>174</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>175</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>176</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>177</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>178</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>181</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>182</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>185</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>186</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>191</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>192</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>193</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>194</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>195</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>196</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>197</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>198</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>199</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>203</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>204</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>205</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>206</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>207</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>208</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>209</v>
       </c>
@@ -4757,12 +4757,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>211</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>212</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>215</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>216</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>217</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>218</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>219</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>220</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>221</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>222</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>223</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>224</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>225</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>226</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>227</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>231</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>232</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>233</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>234</v>
       </c>
@@ -5142,12 +5142,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>236</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>237</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>238</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>239</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>240</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>241</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>242</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>245</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>246</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>247</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>248</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>253</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>256</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>257</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>258</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>259</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>261</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>262</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>263</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>264</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>265</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>268</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>269</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>270</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>272</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>275</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>276</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>277</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>278</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>279</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>280</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>283</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>284</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>285</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>286</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>287</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>288</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>289</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>291</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>292</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>293</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>294</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>295</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>296</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>297</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>304</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>305</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>309</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>313</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>314</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>318</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>321</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>324</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>325</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>326</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>327</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>328</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>329</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>334</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>335</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>340</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>343</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>344</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>346</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>347</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>350</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>351</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>352</v>
       </c>
@@ -6600,22 +6600,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEB1A02-8391-432D-91F9-5DA313B48761}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.59765625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
     <col min="9" max="9" width="99" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="95.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="95.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>81</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>85</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>107</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>108</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>119</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -7581,7 +7581,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>132</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>135</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>138</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>139</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>143</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -7857,7 +7857,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>149</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>152</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>155</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>157</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>158</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>165</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>167</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>170</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>172</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>173</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>174</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>176</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>181</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>185</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>194</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>197</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>198</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>204</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>206</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>210</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>215</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>217</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>224</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>234</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>235</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>236</v>
       </c>
@@ -8509,7 +8509,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>237</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>246</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>257</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>262</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>275</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>278</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>283</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>284</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>285</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>286</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>287</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>291</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>292</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>293</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>294</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>304</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>309</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>327</v>
       </c>
@@ -8899,7 +8899,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>328</v>
       </c>
@@ -8925,7 +8925,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>344</v>
       </c>
@@ -8954,7 +8954,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>346</v>
       </c>
@@ -8977,7 +8977,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>347</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>351</v>
       </c>

</xml_diff>